<commit_message>
Déplacement des fichiers pour remise 2
</commit_message>
<xml_diff>
--- a/Template Excel.xlsx
+++ b/Template Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Front Page" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{9D97C324-AA19-FF42-9C1E-C2CBFE7A4C41}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="604" activeSheetId="3"/>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{9D97C324-AA19-FF42-9C1E-C2CBFE7A4C41}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="604" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -65,9 +65,6 @@
     <t>Faculté de génie</t>
   </si>
   <si>
-    <t>Gestion des risques</t>
-  </si>
-  <si>
     <t>Conception d’un système asservi (GE)</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>Gabriel Martin-Hardy - marg2121 –</t>
   </si>
   <si>
-    <t>Sherbrooke – 9 juin 2016</t>
-  </si>
-  <si>
     <t>Historique des versions</t>
   </si>
   <si>
@@ -147,6 +141,12 @@
   </si>
   <si>
     <t>Toute</t>
+  </si>
+  <si>
+    <t>Titre</t>
+  </si>
+  <si>
+    <t>Sherbrooke – Date 2016</t>
   </si>
 </sst>
 </file>
@@ -576,11 +576,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2104786448"/>
-        <c:axId val="-2106567008"/>
+        <c:axId val="-2143662688"/>
+        <c:axId val="-2143655376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2104786448"/>
+        <c:axId val="-2143662688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -630,7 +630,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2106567008"/>
+        <c:crossAx val="-2143655376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -638,7 +638,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106567008"/>
+        <c:axId val="-2143655376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,7 +691,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2104786448"/>
+        <c:crossAx val="-2143662688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -797,11 +797,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2105775488"/>
-        <c:axId val="-2103058432"/>
+        <c:axId val="-2142639152"/>
+        <c:axId val="-2142636368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2105775488"/>
+        <c:axId val="-2142639152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +810,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103058432"/>
+        <c:crossAx val="-2142636368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2103058432"/>
+        <c:axId val="-2142636368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105775488"/>
+        <c:crossAx val="-2142639152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1058,11 +1058,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="-2103058976"/>
-        <c:axId val="-2105793808"/>
+        <c:axId val="-2143514352"/>
+        <c:axId val="-2143509280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2103058976"/>
+        <c:axId val="-2143514352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,7 +1091,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105793808"/>
+        <c:crossAx val="-2143509280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1099,7 +1099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105793808"/>
+        <c:axId val="-2143509280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103058976"/>
+        <c:crossAx val="-2143514352"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1252,8 +1252,15 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E9109AF5-7FC1-E142-B58C-6BB9D5A8FC5D}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{E4E877E9-B042-1F40-A704-424868C2232F}" diskRevisions="1" revisionId="3" version="2">
   <header guid="{E9109AF5-7FC1-E142-B58C-6BB9D5A8FC5D}" dateTime="2016-06-29T15:05:12" maxSheetId="4" userName="Microsoft Office User" r:id="rId1">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E4E877E9-B042-1F40-A704-424868C2232F}" dateTime="2016-07-05T10:21:53" maxSheetId="4" userName="Microsoft Office User" r:id="rId2" minRId="1" maxRId="2">
     <sheetIdMap count="3">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -1265,6 +1272,41 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1">
+    <oc r="D10" t="inlineStr">
+      <is>
+        <t>Gestion des risques</t>
+      </is>
+    </oc>
+    <nc r="D10" t="inlineStr">
+      <is>
+        <t>Titre</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="2" sId="1">
+    <oc r="D38" t="inlineStr">
+      <is>
+        <t>Sherbrooke – 9 juin 2016</t>
+      </is>
+    </oc>
+    <nc r="D38" t="inlineStr">
+      <is>
+        <t>Sherbrooke – Date 2016</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{9D97C324-AA19-FF42-9C1E-C2CBFE7A4C41}" action="delete"/>
+  <rdn rId="0" localSheetId="3" customView="1" name="Z_9D97C324_AA19_FF42_9C1E_C2CBFE7A4C41_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>Histogramme!$B$1:$C$1005</formula>
+    <oldFormula>Histogramme!$B$1:$C$1005</oldFormula>
+  </rdn>
+  <rcv guid="{9D97C324-AA19-FF42-9C1E-C2CBFE7A4C41}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1560,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:F56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1581,22 +1623,22 @@
     </row>
     <row r="10" spans="4:4" ht="25" x14ac:dyDescent="0.2">
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
@@ -1604,72 +1646,72 @@
     </row>
     <row r="20" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D20" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D27" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D30" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D32" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D33" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D34" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D38" s="2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1677,36 +1719,36 @@
     </row>
     <row r="50" spans="2:6" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="E50" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="F50" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="E51" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1746,8 +1788,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9D97C324-AA19-FF42-9C1E-C2CBFE7A4C41}">
-      <selection activeCell="H9" sqref="H9"/>
+    <customSheetView guid="{9D97C324-AA19-FF42-9C1E-C2CBFE7A4C41}" topLeftCell="A24">
+      <selection activeCell="D39" sqref="D39"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -1921,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>

</xml_diff>